<commit_message>
continuing work on vignette
</commit_message>
<xml_diff>
--- a/xrf_setup.xlsx
+++ b/xrf_setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Swaglife/Desktop/XRF package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Dropbox\XRF_AeN\package\xrfr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC500A-AC7B-C745-BF75-FCA6B52A9D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{735762B7-C716-41B2-820E-5F53AB7E96E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{3B588B98-0B24-F744-A290-1B363CEAA379}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3B588B98-0B24-F744-A290-1B363CEAA379}"/>
   </bookViews>
   <sheets>
     <sheet name="Infofile1" sheetId="4" r:id="rId1"/>
@@ -126,21 +126,12 @@
     <t>Sr</t>
   </si>
   <si>
-    <t>ANO</t>
-  </si>
-  <si>
-    <t>GFF</t>
-  </si>
-  <si>
     <t>MolarW</t>
   </si>
   <si>
     <t>Drift_2019</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
     <t>DL_PC</t>
   </si>
   <si>
@@ -172,6 +163,15 @@
   </si>
   <si>
     <t>Drfit_2018</t>
+  </si>
+  <si>
+    <t>CC_PC</t>
+  </si>
+  <si>
+    <t>CC_ANO</t>
+  </si>
+  <si>
+    <t>CC_GFF</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,68 +565,68 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -679,7 +679,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -732,7 +732,7 @@
         <v>12.42</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -785,7 +785,7 @@
         <v>4.72</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
         <v>35.94</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -891,7 +891,7 @@
         <v>72.11</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -935,7 +935,7 @@
         <v>104.2</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -988,7 +988,7 @@
         <v>322.39999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>28.07</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>28.07</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>28.07</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>404.3</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>240.4</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
small changes in the code
</commit_message>
<xml_diff>
--- a/xrf_setup.xlsx
+++ b/xrf_setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Dropbox\XRF_AeN\package\xrfr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{735762B7-C716-41B2-820E-5F53AB7E96E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBB14F4-D4D5-42FA-9810-EE9199475689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3B588B98-0B24-F744-A290-1B363CEAA379}"/>
   </bookViews>
@@ -165,13 +165,13 @@
     <t>Drfit_2018</t>
   </si>
   <si>
-    <t>CC_PC</t>
-  </si>
-  <si>
-    <t>CC_ANO</t>
-  </si>
-  <si>
-    <t>CC_GFF</t>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>GFF</t>
   </si>
 </sst>
 </file>

</xml_diff>